<commit_message>
subentity migration fully functional
</commit_message>
<xml_diff>
--- a/Item_Types_Migration.xlsx
+++ b/Item_Types_Migration.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,7 +447,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>name=Type,dataType=text,updateCriteria=trueFighting WeaponFighting WeaponFighting WeaponFighting WeaponFighting WeaponFighting WeaponRanged WeaponShieldArmorArmorAccessoryArmorArmorArmorFighting WeaponFighting WeaponFighting WeaponRanged WeaponRanged WeaponRanged WeaponRanged WeaponRanged WeaponRanged WeaponShieldAccessoryAccessoryAccessoryConsumableConsumableConsumableConsumableConsumableConsumable</t>
+          <t>name=Type,dataType=text,updateCriteria=true</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -462,13 +462,91 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>TypeFighting WeaponFighting WeaponFighting WeaponFighting WeaponFighting WeaponFighting WeaponRanged WeaponShieldArmorArmorAccessoryArmorArmorArmorFighting WeaponFighting WeaponFighting WeaponRanged WeaponRanged WeaponRanged WeaponRanged WeaponRanged WeaponRanged WeaponShieldAccessoryAccessoryAccessoryConsumableConsumableConsumableConsumableConsumableConsumable</t>
+          <t>Type</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>visibilityGroups</t>
         </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Fighting Weapon</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Ranged Weapon</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Shield</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Armor</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Accessory</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Consumable</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>